<commit_message>
valid login logout test
</commit_message>
<xml_diff>
--- a/data/actiTIME.xlsx
+++ b/data/actiTIME.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\b84framework\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sabarisha\workspace\b84framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB3B270-D384-4DAC-A161-D617DD62E326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE70E250-A00D-41FA-B15D-413F065AC633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1830" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="ValidLoginLogout" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Password</t>
   </si>
@@ -362,13 +363,13 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -376,7 +377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -393,13 +394,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC8931D-A836-43E0-8540-BEDF5150E8A3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -407,12 +408,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE83B4-D0D5-4427-AE26-D1C4EFF7252A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>